<commit_message>
Mark ZWNL 1967 as finished
</commit_message>
<xml_diff>
--- a/zwnl-2009.xlsx
+++ b/zwnl-2009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10837D07-B9D6-4322-9C36-27EA4F8137B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F7A3E9-5858-4A39-BF89-47B90F2097C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3953" windowWidth="15248" windowHeight="11647" xr2:uid="{BDA33543-83AF-4D7C-906F-E05D921AB472}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>Naam</t>
   </si>
@@ -441,7 +441,10 @@
 - Ddr</t>
   </si>
   <si>
-    <t>Audio?</t>
+    <t>Ambient audio?</t>
+  </si>
+  <si>
+    <t>Omroep?</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A56F8E-D833-4C7F-9673-0AFFF960D58F}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1057,6 +1060,14 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[2461] Fix rood sein inrijder Rsd
</commit_message>
<xml_diff>
--- a/zwnl-2009.xlsx
+++ b/zwnl-2009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F7A3E9-5858-4A39-BF89-47B90F2097C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12F7457-1E4B-418B-8DC0-CCBC5DB8766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3953" windowWidth="15248" windowHeight="11647" xr2:uid="{BDA33543-83AF-4D7C-906F-E05D921AB472}"/>
   </bookViews>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A56F8E-D833-4C7F-9673-0AFFF960D58F}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -878,7 +878,7 @@
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>